<commit_message>
i added my interesting IPs to the excel normalization :)
</commit_message>
<xml_diff>
--- a/manual/jb/jb_Investigation_results.xlsx
+++ b/manual/jb/jb_Investigation_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Downloads/Investigation_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joarbels\projects\let-me-out\manual\jb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B256EB-B352-1244-9567-7D703BF3171D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016A5977-E8CF-4499-89E7-3B2455570B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munkalap1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>IP address</t>
   </si>
@@ -128,6 +128,105 @@
   </si>
   <si>
     <t>Please upload your findings to this table. There is an example row (yellow background). Use different background colour please.</t>
+  </si>
+  <si>
+    <t>80.209.64.86</t>
+  </si>
+  <si>
+    <t>FIBIANET.DK </t>
+  </si>
+  <si>
+    <t>Fibia P/S</t>
+  </si>
+  <si>
+    <t>FIBIA P/S</t>
+  </si>
+  <si>
+    <t>Fixed Line ISP</t>
+  </si>
+  <si>
+    <t>Haslev, Sjaelland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dnsbl.spfbl.net </t>
+  </si>
+  <si>
+    <r>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> / UDP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 19132 / UDP, 25565 / TCP, 8333</t>
+    </r>
+  </si>
+  <si>
+    <t>virustotal: N/A, abuseipdb: N/A</t>
+  </si>
+  <si>
+    <t>80.209.0.0/17</t>
+  </si>
+  <si>
+    <t>MC Server Bedrock and Vanilla</t>
+  </si>
+  <si>
+    <t>files and DNS:Bitcoin and Bither</t>
+  </si>
+  <si>
+    <t>Miner</t>
+  </si>
+  <si>
+    <t>188.228.61.163</t>
+  </si>
+  <si>
+    <t>188.228.0.0/17</t>
+  </si>
+  <si>
+    <t>Altibox AS</t>
+  </si>
+  <si>
+    <t>Skanderborg, Midtjylland, (Engsøparken 141)</t>
+  </si>
+  <si>
+    <t>Spamhaus ZEN, dnsbl.spfbl.net</t>
+  </si>
+  <si>
+    <t>virustotal: -3???, abuseipdb: 16%</t>
+  </si>
+  <si>
+    <t>Port scan, Bruteforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">443 / TCP, 1723 / TCP, 7777 / TCP, 8443 / TCP, 8888 / TCP </t>
+  </si>
+  <si>
+    <t>ALTIBOX.NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router login HTTP 200, </t>
+  </si>
+  <si>
+    <t>ASUS Wireless Router RT-N66U</t>
+  </si>
+  <si>
+    <t>No, I think he ip owner is malicious</t>
+  </si>
+  <si>
+    <t>Mirai botnet, huawei exploit, web crawl</t>
   </si>
 </sst>
 </file>
@@ -137,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +261,58 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF707070"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF20242C"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,10 +368,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -228,8 +380,29 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,33 +619,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:R6"/>
+  <dimension ref="A3:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
-    <col min="14" max="14" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="49" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -492,7 +666,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -510,7 +684,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +740,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -620,12 +794,110 @@
       </c>
       <c r="R6" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:P4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K7" r:id="rId1" display="https://www.shodan.io/domain/fibianet.dk" xr:uid="{2B8DE7B6-567A-4DD0-A20A-F832E881679B}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.shodan.io/search?query=isp%3A%22Altibox+AS%22" xr:uid="{D5707E4A-C6BC-434F-A632-CE52CC568526}"/>
+    <hyperlink ref="K8" r:id="rId3" display="https://www.shodan.io/domain/altibox.net" xr:uid="{50AB756E-8249-49F6-A100-6E3FCA34606D}"/>
+    <hyperlink ref="N8" r:id="rId4" display="https://www.shodan.io/search?query=product%3A%22ASUS+Wireless+Router+RT-N66U%22" xr:uid="{74E0EB65-CC20-4FE3-96F2-48AC08D0C363}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>